<commit_message>
select R_Addin areas when selecting Rdefinitions remove diagrams consistently add refresh button for Rdefinitions improved Doc refactor Workbook_Activate and Workbook_Save
</commit_message>
<xml_diff>
--- a/testDocumentationRAddin.xlsx
+++ b/testDocumentationRAddin.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="15180" yWindow="150" windowWidth="5040" windowHeight="7470" activeTab="1"/>
+    <workbookView xWindow="15180" yWindow="150" windowWidth="5040" windowHeight="7470"/>
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="1" r:id="rId1"/>
@@ -12,22 +12,22 @@
   </sheets>
   <definedNames>
     <definedName name="R_Addin" localSheetId="1">Input_Toy!$J$1:$L$5</definedName>
-    <definedName name="R_Addin">Input!$J$11:$L$15</definedName>
+    <definedName name="R_Addin">Input!$J$15:$L$19</definedName>
     <definedName name="R_AddinAnotherDef" localSheetId="1">Input_Toy!$J$7:$L$12</definedName>
-    <definedName name="R_AddinAnotherDef">Input!$M$11:$O$15</definedName>
+    <definedName name="R_AddinAnotherDef">Input!$M$15:$O$19</definedName>
     <definedName name="test_in" localSheetId="1">Input_Toy!$B$1:$H$3</definedName>
     <definedName name="test_in">Input!$B$1:$H$306</definedName>
     <definedName name="test_out" localSheetId="1">Input_Toy!$A$1:$A$3</definedName>
     <definedName name="test_out">Input!$A$2:$A$49</definedName>
     <definedName name="testdiagram" localSheetId="1">Input_Toy!$J$17</definedName>
-    <definedName name="testdiagram">Input!$J$19</definedName>
+    <definedName name="testdiagram">Input!$J$23</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1899" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1903" uniqueCount="38">
   <si>
     <t/>
   </si>
@@ -83,25 +83,7 @@
     <t>in4</t>
   </si>
   <si>
-    <t>Define Rscript interactions (Rdefinitions):</t>
-  </si>
-  <si>
-    <t>3 column area (1st col: definition type, 2nd: definition value, 3rd: definition path)</t>
-  </si>
-  <si>
-    <t>possible types: rexec, dir, script, arg (R input objects), res (R output objects), diag (R output diagrams)</t>
-  </si>
-  <si>
-    <t>Area name can be Workbook global or worksheet local</t>
-  </si>
-  <si>
-    <t>Rdefinition area name always starts with R_Addin and has an optional postfix as description of the definition</t>
-  </si>
-  <si>
     <t>the worksheet name (for worksheet local names) or the workbook name (for workbook global names) is prepended to the postfix definition description</t>
-  </si>
-  <si>
-    <t>The range names that are referred in arg, res and diag types are also either workbook global or worksheet local (having the worksheet name + ! in front of the name)</t>
   </si>
   <si>
     <t>So for the 4 areas defined in this test workbook there should be 4 entries in the Rdefinition dropdown: Input_toy, test.xlsm, Input_toyAnotherDef, test.xlsmAnotherDef</t>
@@ -130,6 +112,36 @@
   <si>
     <t>testStartRscript.cmd</t>
   </si>
+  <si>
+    <t>Absolute Paths in dir or the definition path column are defined by starting with \\ or X:\ (X being a drive letter)</t>
+  </si>
+  <si>
+    <t>rexec is the full path to an executable being able to run the script in line "script" (usually Rscript.exe). It is only needed when overriding the ExePath in the AppSettings in the Raddin-AddIn-packed.xll.config file.</t>
+  </si>
+  <si>
+    <t>When running cmd shell files a special entry "cmd" is used for rexec.</t>
+  </si>
+  <si>
+    <t>Define Rscript interactions (Rdefinitions) using a 3 column named area (1st col: definition type, 2nd: definition value, 3rd: definition path):</t>
+  </si>
+  <si>
+    <t>Rdefinition area name must start with R_Addin and can have an optional postfix as an additional description of the definition</t>
+  </si>
+  <si>
+    <t>An area name can be Workbook global or worksheet local, the first Rdefinition area is being taken as the default definition (used for running when not selecting a Rdefinition)</t>
+  </si>
+  <si>
+    <t>1st column: definition types, possible types are rexec, dir, script, arg (R input objects, txt files), res (R output objects, txt files) and diag (R output diagrams, png format)</t>
+  </si>
+  <si>
+    <t>2nd column: definition values, for rexec, dir and script this is simply the path/name of the executable/Rdefinition directory/script.</t>
+  </si>
+  <si>
+    <t>For arg, res and diag these are range names referring to the respective ranges to be taken as arg, res or diag target in the excel workbook.</t>
+  </si>
+  <si>
+    <t>The range names that are referred in arg, res and diag types can also be either workbook global (having no ! in front of the name) or worksheet local (having the worksheet name + ! in front of the name)</t>
+  </si>
 </sst>
 </file>
 
@@ -141,7 +153,7 @@
     <numFmt numFmtId="166" formatCode="0.00000"/>
     <numFmt numFmtId="167" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -159,6 +171,12 @@
       <family val="2"/>
     </font>
     <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -189,7 +207,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -198,6 +216,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Komma 2" xfId="3"/>
@@ -259,13 +278,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -592,8 +611,8 @@
   <sheetPr codeName="eingabe"/>
   <dimension ref="A1:O306"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -626,8 +645,8 @@
       <c r="H1" t="s">
         <v>13</v>
       </c>
-      <c r="J1" t="s">
-        <v>18</v>
+      <c r="J1" s="8" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
@@ -657,7 +676,7 @@
       </c>
       <c r="I2" s="7"/>
       <c r="J2" s="7" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
@@ -687,7 +706,7 @@
       </c>
       <c r="I3" s="7"/>
       <c r="J3" s="7" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
@@ -717,7 +736,7 @@
       </c>
       <c r="I4" s="7"/>
       <c r="J4" s="7" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
@@ -747,7 +766,7 @@
       </c>
       <c r="I5" s="7"/>
       <c r="J5" s="7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
@@ -776,9 +795,6 @@
         <v>0.28749999999999998</v>
       </c>
       <c r="I6" s="7"/>
-      <c r="J6" s="7" t="s">
-        <v>23</v>
-      </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7">
@@ -807,10 +823,8 @@
       </c>
       <c r="I7" s="7"/>
       <c r="J7" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="L7" s="7"/>
-      <c r="M7" s="7"/>
+        <v>34</v>
+      </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8">
@@ -839,10 +853,8 @@
       </c>
       <c r="I8" s="7"/>
       <c r="J8" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="L8" s="7"/>
-      <c r="M8" s="7"/>
+        <v>29</v>
+      </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9">
@@ -870,6 +882,11 @@
         <v>1.61E-2</v>
       </c>
       <c r="I9" s="7"/>
+      <c r="J9" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="L9" s="7"/>
+      <c r="M9" s="7"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10">
@@ -897,6 +914,11 @@
         <v>3.1099999999999999E-2</v>
       </c>
       <c r="I10" s="7"/>
+      <c r="J10" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11">
@@ -924,18 +946,11 @@
         <v>0.63400000000000001</v>
       </c>
       <c r="I11" s="7"/>
-      <c r="J11" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="K11" t="s">
-        <v>29</v>
-      </c>
-      <c r="M11" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="N11" t="s">
-        <v>3</v>
-      </c>
+      <c r="J11" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="L11" s="7"/>
+      <c r="M11" s="7"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12">
@@ -963,21 +978,11 @@
         <v>0.5706</v>
       </c>
       <c r="I12" s="7"/>
-      <c r="J12" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="K12" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="M12" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="N12" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="O12" t="s">
-        <v>30</v>
-      </c>
+      <c r="J12" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="L12" s="7"/>
+      <c r="M12" s="7"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13">
@@ -1005,20 +1010,8 @@
         <v>2.4E-2</v>
       </c>
       <c r="I13" s="7"/>
-      <c r="J13" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="K13" t="s">
-        <v>9</v>
-      </c>
-      <c r="M13" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="N13" t="s">
-        <v>9</v>
-      </c>
-      <c r="O13" t="s">
-        <v>30</v>
+      <c r="J13" s="7" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
@@ -1047,21 +1040,6 @@
         <v>2.4E-2</v>
       </c>
       <c r="I14" s="7"/>
-      <c r="J14" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="K14" t="s">
-        <v>10</v>
-      </c>
-      <c r="M14" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="N14" t="s">
-        <v>10</v>
-      </c>
-      <c r="O14" t="s">
-        <v>30</v>
-      </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15">
@@ -1089,20 +1067,17 @@
         <v>1.38E-2</v>
       </c>
       <c r="I15" s="7"/>
-      <c r="J15" s="3" t="s">
-        <v>7</v>
+      <c r="J15" s="4" t="s">
+        <v>2</v>
       </c>
       <c r="K15" t="s">
-        <v>4</v>
-      </c>
-      <c r="M15" s="3" t="s">
-        <v>7</v>
+        <v>23</v>
+      </c>
+      <c r="M15" s="4" t="s">
+        <v>2</v>
       </c>
       <c r="N15" t="s">
-        <v>4</v>
-      </c>
-      <c r="O15" t="s">
-        <v>30</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
@@ -1131,11 +1106,23 @@
         <v>0.40250000000000002</v>
       </c>
       <c r="I16" s="7"/>
-      <c r="J16" s="7"/>
-      <c r="L16" s="7"/>
-      <c r="M16" s="7"/>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="J16" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M16" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="N16" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="O16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>6</v>
       </c>
@@ -1161,11 +1148,23 @@
         <v>0.40250000000000002</v>
       </c>
       <c r="I17" s="7"/>
-      <c r="J17" s="7"/>
-      <c r="L17" s="7"/>
-      <c r="M17" s="7"/>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="J17" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="K17" t="s">
+        <v>9</v>
+      </c>
+      <c r="M17" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="N17" t="s">
+        <v>9</v>
+      </c>
+      <c r="O17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>7</v>
       </c>
@@ -1191,11 +1190,23 @@
         <v>1.2699999999999999E-2</v>
       </c>
       <c r="I18" s="7"/>
-      <c r="J18" s="7"/>
-      <c r="L18" s="7"/>
-      <c r="M18" s="7"/>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="J18" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="K18" t="s">
+        <v>10</v>
+      </c>
+      <c r="M18" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="N18" t="s">
+        <v>10</v>
+      </c>
+      <c r="O18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>7</v>
       </c>
@@ -1221,11 +1232,23 @@
         <v>1.2699999999999999E-2</v>
       </c>
       <c r="I19" s="7"/>
-      <c r="J19" s="7"/>
-      <c r="L19" s="7"/>
-      <c r="M19" s="7"/>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="J19" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K19" t="s">
+        <v>4</v>
+      </c>
+      <c r="M19" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="N19" t="s">
+        <v>4</v>
+      </c>
+      <c r="O19" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>8</v>
       </c>
@@ -1255,7 +1278,7 @@
       <c r="L20" s="7"/>
       <c r="M20" s="7"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>9</v>
       </c>
@@ -1285,7 +1308,7 @@
       <c r="L21" s="7"/>
       <c r="M21" s="7"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>9</v>
       </c>
@@ -1315,7 +1338,7 @@
       <c r="L22" s="7"/>
       <c r="M22" s="7"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>10</v>
       </c>
@@ -1345,7 +1368,7 @@
       <c r="L23" s="7"/>
       <c r="M23" s="7"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>10</v>
       </c>
@@ -1375,7 +1398,7 @@
       <c r="L24" s="7"/>
       <c r="M24" s="7"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>3</v>
       </c>
@@ -1405,7 +1428,7 @@
       <c r="L25" s="7"/>
       <c r="M25" s="7"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>3</v>
       </c>
@@ -1435,7 +1458,7 @@
       <c r="L26" s="7"/>
       <c r="M26" s="7"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>3</v>
       </c>
@@ -1465,7 +1488,7 @@
       <c r="L27" s="7"/>
       <c r="M27" s="7"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>3</v>
       </c>
@@ -1495,7 +1518,7 @@
       <c r="L28" s="7"/>
       <c r="M28" s="7"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>4</v>
       </c>
@@ -1525,7 +1548,7 @@
       <c r="L29" s="7"/>
       <c r="M29" s="7"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>4</v>
       </c>
@@ -1555,7 +1578,7 @@
       <c r="L30" s="7"/>
       <c r="M30" s="7"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>4</v>
       </c>
@@ -1585,7 +1608,7 @@
       <c r="L31" s="7"/>
       <c r="M31" s="7"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>4</v>
       </c>
@@ -2095,7 +2118,7 @@
       <c r="L48" s="7"/>
       <c r="M48" s="7"/>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A49"/>
       <c r="B49" t="s">
         <v>0</v>
@@ -2120,8 +2143,10 @@
       </c>
       <c r="I49" s="7"/>
       <c r="J49" s="7"/>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="L49" s="7"/>
+      <c r="M49" s="7"/>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B50" t="s">
         <v>0</v>
       </c>
@@ -2144,8 +2169,11 @@
         <v>0</v>
       </c>
       <c r="I50" s="7"/>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J50" s="7"/>
+      <c r="L50" s="7"/>
+      <c r="M50" s="7"/>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B51" t="s">
         <v>0</v>
       </c>
@@ -2167,8 +2195,11 @@
       <c r="H51" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J51" s="7"/>
+      <c r="L51" s="7"/>
+      <c r="M51" s="7"/>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B52" t="s">
         <v>0</v>
       </c>
@@ -2190,8 +2221,11 @@
       <c r="H52" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J52" s="7"/>
+      <c r="L52" s="7"/>
+      <c r="M52" s="7"/>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
         <v>0</v>
       </c>
@@ -2213,8 +2247,9 @@
       <c r="H53" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J53" s="7"/>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
         <v>0</v>
       </c>
@@ -2237,7 +2272,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B55" t="s">
         <v>0</v>
       </c>
@@ -2260,7 +2295,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B56" t="s">
         <v>0</v>
       </c>
@@ -2283,7 +2318,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B57" t="s">
         <v>0</v>
       </c>
@@ -2306,7 +2341,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B58" t="s">
         <v>0</v>
       </c>
@@ -2329,7 +2364,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B59" t="s">
         <v>0</v>
       </c>
@@ -2352,7 +2387,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B60" t="s">
         <v>0</v>
       </c>
@@ -2375,7 +2410,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B61" t="s">
         <v>0</v>
       </c>
@@ -2398,7 +2433,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B62" t="s">
         <v>0</v>
       </c>
@@ -2421,7 +2456,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B63" t="s">
         <v>0</v>
       </c>
@@ -2444,7 +2479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B64" t="s">
         <v>0</v>
       </c>
@@ -8048,7 +8083,7 @@
   <sheetPr codeName="eingabeToy"/>
   <dimension ref="A1:K47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection sqref="A1:A47"/>
     </sheetView>
   </sheetViews>
@@ -8156,7 +8191,7 @@
         <v>6</v>
       </c>
       <c r="K3" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
@@ -8165,7 +8200,7 @@
         <v>5</v>
       </c>
       <c r="K4" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
@@ -8174,7 +8209,7 @@
         <v>7</v>
       </c>
       <c r="K5" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
@@ -8184,10 +8219,10 @@
       <c r="A7"/>
       <c r="C7" s="6"/>
       <c r="J7" s="4" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="K7" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
@@ -8205,7 +8240,7 @@
         <v>1</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
@@ -8214,7 +8249,7 @@
         <v>6</v>
       </c>
       <c r="K10" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
@@ -8223,7 +8258,7 @@
         <v>5</v>
       </c>
       <c r="K11" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
@@ -8232,7 +8267,7 @@
         <v>7</v>
       </c>
       <c r="K12" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
added exception handling when deleting previous diagrams/results
</commit_message>
<xml_diff>
--- a/testDocumentationRAddin.xlsx
+++ b/testDocumentationRAddin.xlsx
@@ -12,22 +12,22 @@
   </sheets>
   <definedNames>
     <definedName name="R_Addin" localSheetId="1">Input_Toy!$J$1:$L$5</definedName>
-    <definedName name="R_Addin">Input!$J$15:$L$19</definedName>
+    <definedName name="R_Addin">Input!$J$19:$L$23</definedName>
     <definedName name="R_AddinAnotherDef" localSheetId="1">Input_Toy!$J$7:$L$12</definedName>
-    <definedName name="R_AddinAnotherDef">Input!$M$15:$O$19</definedName>
-    <definedName name="test_in" localSheetId="1">Input_Toy!$B$1:$H$3</definedName>
+    <definedName name="R_AddinAnotherDef">Input!$M$19:$O$23</definedName>
+    <definedName name="test_in" localSheetId="1">Input_Toy!$B$1:$H$4</definedName>
     <definedName name="test_in">Input!$B$1:$H$306</definedName>
-    <definedName name="test_out" localSheetId="1">Input_Toy!$A$1:$A$3</definedName>
+    <definedName name="test_out" localSheetId="1">Input_Toy!$A$2:$A$4</definedName>
     <definedName name="test_out">Input!$A$2:$A$49</definedName>
     <definedName name="testdiagram" localSheetId="1">Input_Toy!$J$17</definedName>
-    <definedName name="testdiagram">Input!$J$23</definedName>
+    <definedName name="testdiagram">Input!$J$26</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1903" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1883" uniqueCount="43">
   <si>
     <t/>
   </si>
@@ -122,9 +122,6 @@
     <t>When running cmd shell files a special entry "cmd" is used for rexec.</t>
   </si>
   <si>
-    <t>Define Rscript interactions (Rdefinitions) using a 3 column named area (1st col: definition type, 2nd: definition value, 3rd: definition path):</t>
-  </si>
-  <si>
     <t>Rdefinition area name must start with R_Addin and can have an optional postfix as an additional description of the definition</t>
   </si>
   <si>
@@ -141,6 +138,24 @@
   </si>
   <si>
     <t>The range names that are referred in arg, res and diag types can also be either workbook global (having no ! in front of the name) or worksheet local (having the worksheet name + ! in front of the name)</t>
+  </si>
+  <si>
+    <t>The definitions are loaded inot the Rdefinition dropdown either on opening/activating a Workbook with above named areas or by pressing "refresh Rdefinitions" on the R Addin Ribbon Tab.</t>
+  </si>
+  <si>
+    <t>R Addin provides an easy way to define and run R script interactions started from Excel.</t>
+  </si>
+  <si>
+    <t>Running an R script is simply done by selecting the appropriate Rdefinition and pressing "run this Rdefinition" on the R Addin Ribbon Tab.</t>
+  </si>
+  <si>
+    <t>Selecting the Rdefinition highlights the specified definition area (see below).</t>
+  </si>
+  <si>
+    <t>How to define Rscript interactions (Rdefinitions) using a 3 column named area (1st col: definition type, 2nd: definition value, 3rd: definition path):</t>
+  </si>
+  <si>
+    <t>result:</t>
   </si>
 </sst>
 </file>
@@ -278,13 +293,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>53</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -309,6 +324,99 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3295650" y="2914650"/>
+          <a:ext cx="4572000" cy="4572000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="testdiagram.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4010025" y="4048125"/>
+          <a:ext cx="4572000" cy="4572000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="testdiagram.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3009900" y="2590800"/>
           <a:ext cx="4572000" cy="4572000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -612,18 +720,18 @@
   <dimension ref="A1:O306"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="R19" sqref="R19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.85546875" style="4" customWidth="1"/>
-    <col min="2" max="6" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="5.42578125" customWidth="1"/>
     <col min="8" max="8" width="5.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>14</v>
       </c>
@@ -645,28 +753,28 @@
       <c r="H1" t="s">
         <v>13</v>
       </c>
-      <c r="J1" s="8" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="J1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>2</v>
-      </c>
-      <c r="B2">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
+        <v>0.29749999999999999</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0.29749999999999999</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0.40250000000000002</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0.29749999999999999</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0.29749999999999999</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0.40250000000000002</v>
       </c>
       <c r="G2" s="1">
         <v>0.29749999999999999</v>
@@ -675,28 +783,28 @@
         <v>0.40250000000000002</v>
       </c>
       <c r="I2" s="7"/>
-      <c r="J2" s="7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="J2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>3</v>
-      </c>
-      <c r="B3">
-        <v>3</v>
-      </c>
-      <c r="C3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
+        <v>0.30690000000000001</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0.30690000000000001</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0.50719999999999998</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0.30690000000000001</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0.30690000000000001</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0.50719999999999998</v>
       </c>
       <c r="G3" s="1">
         <v>0.30690000000000001</v>
@@ -705,28 +813,28 @@
         <v>0.50719999999999998</v>
       </c>
       <c r="I3" s="7"/>
-      <c r="J3" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="J3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>4</v>
-      </c>
-      <c r="B4">
-        <v>4</v>
-      </c>
-      <c r="C4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4" t="s">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
+        <v>1.04E-2</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1.04E-2</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1.7100000000000001E-2</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1.04E-2</v>
+      </c>
+      <c r="E4" s="1">
+        <v>1.04E-2</v>
+      </c>
+      <c r="F4" s="1">
+        <v>1.7100000000000001E-2</v>
       </c>
       <c r="G4" s="1">
         <v>1.04E-2</v>
@@ -735,28 +843,28 @@
         <v>1.7100000000000001E-2</v>
       </c>
       <c r="I4" s="7"/>
-      <c r="J4" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="J4" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>5</v>
-      </c>
-      <c r="B5">
-        <v>5</v>
-      </c>
-      <c r="C5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5" t="s">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>1</v>
+        <v>5.1000000000000004E-3</v>
+      </c>
+      <c r="B5" s="1">
+        <v>5.1000000000000004E-3</v>
+      </c>
+      <c r="C5" s="1">
+        <v>6.8999999999999999E-3</v>
+      </c>
+      <c r="D5" s="1">
+        <v>5.1000000000000004E-3</v>
+      </c>
+      <c r="E5" s="1">
+        <v>5.1000000000000004E-3</v>
+      </c>
+      <c r="F5" s="1">
+        <v>6.8999999999999999E-3</v>
       </c>
       <c r="G5" s="1">
         <v>5.1000000000000004E-3</v>
@@ -766,27 +874,27 @@
       </c>
       <c r="I5" s="7"/>
       <c r="J5" s="7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>6</v>
-      </c>
-      <c r="B6">
-        <v>6</v>
-      </c>
-      <c r="C6" t="s">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6" t="s">
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <v>1</v>
+        <v>0.21249999999999999</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0.21249999999999999</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0.28749999999999998</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0.21249999999999999</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0.21249999999999999</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0.28749999999999998</v>
       </c>
       <c r="G6" s="1">
         <v>0.21249999999999999</v>
@@ -795,25 +903,28 @@
         <v>0.28749999999999998</v>
       </c>
       <c r="I6" s="7"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="J6" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>7</v>
-      </c>
-      <c r="B7">
-        <v>7</v>
-      </c>
-      <c r="C7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7" t="s">
-        <v>0</v>
-      </c>
-      <c r="F7">
-        <v>1</v>
+        <v>5.4999999999999997E-3</v>
+      </c>
+      <c r="B7" s="1">
+        <v>5.4999999999999997E-3</v>
+      </c>
+      <c r="C7" s="1">
+        <v>8.8999999999999999E-3</v>
+      </c>
+      <c r="D7" s="1">
+        <v>5.4999999999999997E-3</v>
+      </c>
+      <c r="E7" s="1">
+        <v>5.4999999999999997E-3</v>
+      </c>
+      <c r="F7" s="1">
+        <v>8.8999999999999999E-3</v>
       </c>
       <c r="G7" s="1">
         <v>5.4999999999999997E-3</v>
@@ -823,27 +934,27 @@
       </c>
       <c r="I7" s="7"/>
       <c r="J7" s="7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>8</v>
-      </c>
-      <c r="B8">
-        <v>8</v>
-      </c>
-      <c r="C8" t="s">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-      <c r="E8" t="s">
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <v>1</v>
+        <v>8.5000000000000006E-3</v>
+      </c>
+      <c r="B8" s="1">
+        <v>8.5000000000000006E-3</v>
+      </c>
+      <c r="C8" s="1">
+        <v>1.15E-2</v>
+      </c>
+      <c r="D8" s="1">
+        <v>8.5000000000000006E-3</v>
+      </c>
+      <c r="E8" s="1">
+        <v>8.5000000000000006E-3</v>
+      </c>
+      <c r="F8" s="1">
+        <v>1.15E-2</v>
       </c>
       <c r="G8" s="1">
         <v>8.5000000000000006E-3</v>
@@ -853,27 +964,27 @@
       </c>
       <c r="I8" s="7"/>
       <c r="J8" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>9</v>
-      </c>
-      <c r="B9">
-        <v>9</v>
-      </c>
-      <c r="C9" t="s">
-        <v>0</v>
-      </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="E9" t="s">
-        <v>0</v>
-      </c>
-      <c r="F9">
-        <v>1</v>
+        <v>1.1900000000000001E-2</v>
+      </c>
+      <c r="B9" s="1">
+        <v>1.1900000000000001E-2</v>
+      </c>
+      <c r="C9" s="1">
+        <v>1.61E-2</v>
+      </c>
+      <c r="D9" s="1">
+        <v>1.1900000000000001E-2</v>
+      </c>
+      <c r="E9" s="1">
+        <v>1.1900000000000001E-2</v>
+      </c>
+      <c r="F9" s="1">
+        <v>1.61E-2</v>
       </c>
       <c r="G9" s="1">
         <v>1.1900000000000001E-2</v>
@@ -882,30 +993,25 @@
         <v>1.61E-2</v>
       </c>
       <c r="I9" s="7"/>
-      <c r="J9" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="L9" s="7"/>
-      <c r="M9" s="7"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>10</v>
-      </c>
-      <c r="B10">
-        <v>10</v>
-      </c>
-      <c r="C10" t="s">
-        <v>0</v>
-      </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-      <c r="E10" t="s">
-        <v>0</v>
-      </c>
-      <c r="F10">
-        <v>1</v>
+        <v>2.3E-2</v>
+      </c>
+      <c r="B10" s="1">
+        <v>2.3E-2</v>
+      </c>
+      <c r="C10" s="1">
+        <v>3.1099999999999999E-2</v>
+      </c>
+      <c r="D10" s="1">
+        <v>2.3E-2</v>
+      </c>
+      <c r="E10" s="1">
+        <v>2.3E-2</v>
+      </c>
+      <c r="F10" s="1">
+        <v>3.1099999999999999E-2</v>
       </c>
       <c r="G10" s="1">
         <v>2.3E-2</v>
@@ -915,29 +1021,27 @@
       </c>
       <c r="I10" s="7"/>
       <c r="J10" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="L10" s="7"/>
-      <c r="M10" s="7"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>3</v>
-      </c>
-      <c r="B11">
-        <v>3</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-      <c r="E11" t="s">
-        <v>0</v>
-      </c>
-      <c r="F11">
-        <v>1</v>
+        <v>0.3836</v>
+      </c>
+      <c r="B11" s="1">
+        <v>0.3836</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0.63400000000000001</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0.3836</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0.3836</v>
+      </c>
+      <c r="F11" s="1">
+        <v>0.63400000000000001</v>
       </c>
       <c r="G11" s="1">
         <v>0.3836</v>
@@ -947,29 +1051,27 @@
       </c>
       <c r="I11" s="7"/>
       <c r="J11" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="L11" s="7"/>
-      <c r="M11" s="7"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>3</v>
-      </c>
-      <c r="B12">
-        <v>3</v>
-      </c>
-      <c r="C12">
-        <v>2</v>
-      </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-      <c r="E12" t="s">
-        <v>0</v>
-      </c>
-      <c r="F12">
-        <v>1</v>
+        <v>0.34520000000000001</v>
+      </c>
+      <c r="B12" s="1">
+        <v>0.34520000000000001</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0.5706</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0.34520000000000001</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0.34520000000000001</v>
+      </c>
+      <c r="F12" s="1">
+        <v>0.5706</v>
       </c>
       <c r="G12" s="1">
         <v>0.34520000000000001</v>
@@ -979,29 +1081,29 @@
       </c>
       <c r="I12" s="7"/>
       <c r="J12" s="7" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="L12" s="7"/>
       <c r="M12" s="7"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>4</v>
-      </c>
-      <c r="B13">
-        <v>4</v>
-      </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
-      <c r="E13" t="s">
-        <v>0</v>
-      </c>
-      <c r="F13">
-        <v>1</v>
+        <v>1.4500000000000001E-2</v>
+      </c>
+      <c r="B13" s="1">
+        <v>1.4500000000000001E-2</v>
+      </c>
+      <c r="C13" s="1">
+        <v>2.4E-2</v>
+      </c>
+      <c r="D13" s="1">
+        <v>1.4500000000000001E-2</v>
+      </c>
+      <c r="E13" s="1">
+        <v>1.4500000000000001E-2</v>
+      </c>
+      <c r="F13" s="1">
+        <v>2.4E-2</v>
       </c>
       <c r="G13" s="1">
         <v>1.4500000000000001E-2</v>
@@ -1011,27 +1113,29 @@
       </c>
       <c r="I13" s="7"/>
       <c r="J13" s="7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+      <c r="L13" s="7"/>
+      <c r="M13" s="7"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>4</v>
-      </c>
-      <c r="B14">
-        <v>4</v>
-      </c>
-      <c r="C14">
-        <v>2</v>
-      </c>
-      <c r="D14">
-        <v>1</v>
-      </c>
-      <c r="E14" t="s">
-        <v>0</v>
-      </c>
-      <c r="F14">
-        <v>1</v>
+        <v>1.4500000000000001E-2</v>
+      </c>
+      <c r="B14" s="1">
+        <v>1.4500000000000001E-2</v>
+      </c>
+      <c r="C14" s="1">
+        <v>2.4E-2</v>
+      </c>
+      <c r="D14" s="1">
+        <v>1.4500000000000001E-2</v>
+      </c>
+      <c r="E14" s="1">
+        <v>1.4500000000000001E-2</v>
+      </c>
+      <c r="F14" s="1">
+        <v>2.4E-2</v>
       </c>
       <c r="G14" s="1">
         <v>1.4500000000000001E-2</v>
@@ -1040,25 +1144,30 @@
         <v>2.4E-2</v>
       </c>
       <c r="I14" s="7"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="J14" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="L14" s="7"/>
+      <c r="M14" s="7"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>5</v>
-      </c>
-      <c r="B15">
-        <v>5</v>
-      </c>
-      <c r="C15">
-        <v>2</v>
-      </c>
-      <c r="D15">
-        <v>1</v>
-      </c>
-      <c r="E15" t="s">
-        <v>0</v>
-      </c>
-      <c r="F15">
-        <v>1</v>
+        <v>1.0200000000000001E-2</v>
+      </c>
+      <c r="B15" s="1">
+        <v>1.0200000000000001E-2</v>
+      </c>
+      <c r="C15" s="1">
+        <v>1.38E-2</v>
+      </c>
+      <c r="D15" s="1">
+        <v>1.0200000000000001E-2</v>
+      </c>
+      <c r="E15" s="1">
+        <v>1.0200000000000001E-2</v>
+      </c>
+      <c r="F15" s="1">
+        <v>1.38E-2</v>
       </c>
       <c r="G15" s="1">
         <v>1.0200000000000001E-2</v>
@@ -1067,37 +1176,30 @@
         <v>1.38E-2</v>
       </c>
       <c r="I15" s="7"/>
-      <c r="J15" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="K15" t="s">
-        <v>23</v>
-      </c>
-      <c r="M15" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="N15" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="J15" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="L15" s="7"/>
+      <c r="M15" s="7"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>6</v>
-      </c>
-      <c r="B16">
-        <v>6</v>
-      </c>
-      <c r="C16">
-        <v>1</v>
-      </c>
-      <c r="D16">
-        <v>1</v>
-      </c>
-      <c r="E16" t="s">
-        <v>0</v>
-      </c>
-      <c r="F16">
-        <v>1</v>
+        <v>0.29749999999999999</v>
+      </c>
+      <c r="B16" s="1">
+        <v>0.29749999999999999</v>
+      </c>
+      <c r="C16" s="1">
+        <v>0.40250000000000002</v>
+      </c>
+      <c r="D16" s="1">
+        <v>0.29749999999999999</v>
+      </c>
+      <c r="E16" s="1">
+        <v>0.29749999999999999</v>
+      </c>
+      <c r="F16" s="1">
+        <v>0.40250000000000002</v>
       </c>
       <c r="G16" s="1">
         <v>0.29749999999999999</v>
@@ -1106,40 +1208,28 @@
         <v>0.40250000000000002</v>
       </c>
       <c r="I16" s="7"/>
-      <c r="J16" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="K16" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="M16" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="N16" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="O16" t="s">
-        <v>24</v>
+      <c r="J16" s="7" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>6</v>
-      </c>
-      <c r="B17">
-        <v>6</v>
-      </c>
-      <c r="C17">
-        <v>2</v>
-      </c>
-      <c r="D17">
-        <v>1</v>
-      </c>
-      <c r="E17" t="s">
-        <v>0</v>
-      </c>
-      <c r="F17">
-        <v>1</v>
+        <v>0.29749999999999999</v>
+      </c>
+      <c r="B17" s="1">
+        <v>0.29749999999999999</v>
+      </c>
+      <c r="C17" s="1">
+        <v>0.40250000000000002</v>
+      </c>
+      <c r="D17" s="1">
+        <v>0.29749999999999999</v>
+      </c>
+      <c r="E17" s="1">
+        <v>0.29749999999999999</v>
+      </c>
+      <c r="F17" s="1">
+        <v>0.40250000000000002</v>
       </c>
       <c r="G17" s="1">
         <v>0.29749999999999999</v>
@@ -1148,40 +1238,28 @@
         <v>0.40250000000000002</v>
       </c>
       <c r="I17" s="7"/>
-      <c r="J17" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="K17" t="s">
-        <v>9</v>
-      </c>
-      <c r="M17" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="N17" t="s">
-        <v>9</v>
-      </c>
-      <c r="O17" t="s">
-        <v>24</v>
+      <c r="J17" s="7" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>7</v>
-      </c>
-      <c r="B18">
-        <v>7</v>
-      </c>
-      <c r="C18">
-        <v>1</v>
-      </c>
-      <c r="D18">
-        <v>1</v>
-      </c>
-      <c r="E18" t="s">
-        <v>0</v>
-      </c>
-      <c r="F18">
-        <v>1</v>
+        <v>7.7000000000000002E-3</v>
+      </c>
+      <c r="B18" s="1">
+        <v>7.7000000000000002E-3</v>
+      </c>
+      <c r="C18" s="1">
+        <v>1.2699999999999999E-2</v>
+      </c>
+      <c r="D18" s="1">
+        <v>7.7000000000000002E-3</v>
+      </c>
+      <c r="E18" s="1">
+        <v>7.7000000000000002E-3</v>
+      </c>
+      <c r="F18" s="1">
+        <v>1.2699999999999999E-2</v>
       </c>
       <c r="G18" s="1">
         <v>7.7000000000000002E-3</v>
@@ -1190,40 +1268,25 @@
         <v>1.2699999999999999E-2</v>
       </c>
       <c r="I18" s="7"/>
-      <c r="J18" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="K18" t="s">
-        <v>10</v>
-      </c>
-      <c r="M18" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="N18" t="s">
-        <v>10</v>
-      </c>
-      <c r="O18" t="s">
-        <v>24</v>
-      </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>7</v>
-      </c>
-      <c r="B19">
-        <v>7</v>
-      </c>
-      <c r="C19">
-        <v>2</v>
-      </c>
-      <c r="D19">
-        <v>1</v>
-      </c>
-      <c r="E19" t="s">
-        <v>0</v>
-      </c>
-      <c r="F19">
-        <v>1</v>
+        <v>7.7000000000000002E-3</v>
+      </c>
+      <c r="B19" s="1">
+        <v>7.7000000000000002E-3</v>
+      </c>
+      <c r="C19" s="1">
+        <v>1.2699999999999999E-2</v>
+      </c>
+      <c r="D19" s="1">
+        <v>7.7000000000000002E-3</v>
+      </c>
+      <c r="E19" s="1">
+        <v>7.7000000000000002E-3</v>
+      </c>
+      <c r="F19" s="1">
+        <v>1.2699999999999999E-2</v>
       </c>
       <c r="G19" s="1">
         <v>7.7000000000000002E-3</v>
@@ -1232,40 +1295,37 @@
         <v>1.2699999999999999E-2</v>
       </c>
       <c r="I19" s="7"/>
-      <c r="J19" s="3" t="s">
-        <v>7</v>
+      <c r="J19" s="4" t="s">
+        <v>2</v>
       </c>
       <c r="K19" t="s">
-        <v>4</v>
-      </c>
-      <c r="M19" s="3" t="s">
-        <v>7</v>
+        <v>3</v>
+      </c>
+      <c r="M19" s="4" t="s">
+        <v>2</v>
       </c>
       <c r="N19" t="s">
-        <v>4</v>
-      </c>
-      <c r="O19" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>8</v>
-      </c>
-      <c r="B20">
-        <v>8</v>
-      </c>
-      <c r="C20">
-        <v>3</v>
-      </c>
-      <c r="D20">
-        <v>1</v>
-      </c>
-      <c r="E20" t="s">
-        <v>0</v>
-      </c>
-      <c r="F20">
-        <v>1</v>
+        <v>1.1900000000000001E-2</v>
+      </c>
+      <c r="B20" s="1">
+        <v>1.1900000000000001E-2</v>
+      </c>
+      <c r="C20" s="1">
+        <v>1.61E-2</v>
+      </c>
+      <c r="D20" s="1">
+        <v>1.1900000000000001E-2</v>
+      </c>
+      <c r="E20" s="1">
+        <v>1.1900000000000001E-2</v>
+      </c>
+      <c r="F20" s="1">
+        <v>1.61E-2</v>
       </c>
       <c r="G20" s="1">
         <v>1.1900000000000001E-2</v>
@@ -1274,28 +1334,40 @@
         <v>1.61E-2</v>
       </c>
       <c r="I20" s="7"/>
-      <c r="J20" s="7"/>
-      <c r="L20" s="7"/>
-      <c r="M20" s="7"/>
+      <c r="J20" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M20" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="N20" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="O20" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>9</v>
-      </c>
-      <c r="B21">
-        <v>9</v>
-      </c>
-      <c r="C21">
-        <v>3</v>
-      </c>
-      <c r="D21">
-        <v>1</v>
-      </c>
-      <c r="E21" t="s">
-        <v>0</v>
-      </c>
-      <c r="F21">
-        <v>1</v>
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="B21" s="1">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="C21" s="1">
+        <v>2.3E-2</v>
+      </c>
+      <c r="D21" s="1">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="E21" s="1">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="F21" s="1">
+        <v>2.3E-2</v>
       </c>
       <c r="G21" s="1">
         <v>1.7000000000000001E-2</v>
@@ -1304,28 +1376,40 @@
         <v>2.3E-2</v>
       </c>
       <c r="I21" s="7"/>
-      <c r="J21" s="7"/>
-      <c r="L21" s="7"/>
-      <c r="M21" s="7"/>
+      <c r="J21" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="K21" t="s">
+        <v>9</v>
+      </c>
+      <c r="M21" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="N21" t="s">
+        <v>9</v>
+      </c>
+      <c r="O21" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>9</v>
-      </c>
-      <c r="B22">
-        <v>9</v>
-      </c>
-      <c r="C22">
-        <v>6</v>
-      </c>
-      <c r="D22">
-        <v>1</v>
-      </c>
-      <c r="E22" t="s">
-        <v>0</v>
-      </c>
-      <c r="F22">
-        <v>1</v>
+        <v>1.9099999999999999E-2</v>
+      </c>
+      <c r="B22" s="1">
+        <v>1.9099999999999999E-2</v>
+      </c>
+      <c r="C22" s="1">
+        <v>2.5899999999999999E-2</v>
+      </c>
+      <c r="D22" s="1">
+        <v>1.9099999999999999E-2</v>
+      </c>
+      <c r="E22" s="1">
+        <v>1.9099999999999999E-2</v>
+      </c>
+      <c r="F22" s="1">
+        <v>2.5899999999999999E-2</v>
       </c>
       <c r="G22" s="1">
         <v>1.9099999999999999E-2</v>
@@ -1334,28 +1418,40 @@
         <v>2.5899999999999999E-2</v>
       </c>
       <c r="I22" s="7"/>
-      <c r="J22" s="7"/>
-      <c r="L22" s="7"/>
-      <c r="M22" s="7"/>
+      <c r="J22" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="K22" t="s">
+        <v>10</v>
+      </c>
+      <c r="M22" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="N22" t="s">
+        <v>10</v>
+      </c>
+      <c r="O22" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>10</v>
-      </c>
-      <c r="B23">
-        <v>10</v>
-      </c>
-      <c r="C23">
-        <v>8</v>
-      </c>
-      <c r="D23">
-        <v>1</v>
-      </c>
-      <c r="E23" t="s">
-        <v>0</v>
-      </c>
-      <c r="F23">
-        <v>1</v>
+        <v>4.2500000000000003E-2</v>
+      </c>
+      <c r="B23" s="1">
+        <v>4.2500000000000003E-2</v>
+      </c>
+      <c r="C23" s="1">
+        <v>5.7500000000000002E-2</v>
+      </c>
+      <c r="D23" s="1">
+        <v>4.2500000000000003E-2</v>
+      </c>
+      <c r="E23" s="1">
+        <v>4.2500000000000003E-2</v>
+      </c>
+      <c r="F23" s="1">
+        <v>5.7500000000000002E-2</v>
       </c>
       <c r="G23" s="1">
         <v>4.2500000000000003E-2</v>
@@ -1364,28 +1460,40 @@
         <v>5.7500000000000002E-2</v>
       </c>
       <c r="I23" s="7"/>
-      <c r="J23" s="7"/>
-      <c r="L23" s="7"/>
-      <c r="M23" s="7"/>
+      <c r="J23" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K23" t="s">
+        <v>4</v>
+      </c>
+      <c r="M23" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="N23" t="s">
+        <v>4</v>
+      </c>
+      <c r="O23" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>10</v>
-      </c>
-      <c r="B24">
-        <v>10</v>
-      </c>
-      <c r="C24">
-        <v>9</v>
-      </c>
-      <c r="D24">
-        <v>1</v>
-      </c>
-      <c r="E24" t="s">
-        <v>0</v>
-      </c>
-      <c r="F24">
-        <v>1</v>
+        <v>3.8300000000000001E-2</v>
+      </c>
+      <c r="B24" s="1">
+        <v>3.8300000000000001E-2</v>
+      </c>
+      <c r="C24" s="1">
+        <v>5.1799999999999999E-2</v>
+      </c>
+      <c r="D24" s="1">
+        <v>3.8300000000000001E-2</v>
+      </c>
+      <c r="E24" s="1">
+        <v>3.8300000000000001E-2</v>
+      </c>
+      <c r="F24" s="1">
+        <v>5.1799999999999999E-2</v>
       </c>
       <c r="G24" s="1">
         <v>3.8300000000000001E-2</v>
@@ -1400,22 +1508,22 @@
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>3</v>
-      </c>
-      <c r="B25">
-        <v>3</v>
-      </c>
-      <c r="C25">
-        <v>1</v>
-      </c>
-      <c r="D25">
-        <v>1</v>
-      </c>
-      <c r="E25">
-        <v>2</v>
-      </c>
-      <c r="F25">
-        <v>1</v>
+        <v>0.44500000000000001</v>
+      </c>
+      <c r="B25" s="1">
+        <v>0.44500000000000001</v>
+      </c>
+      <c r="C25" s="1">
+        <v>0.73540000000000005</v>
+      </c>
+      <c r="D25" s="1">
+        <v>0.44500000000000001</v>
+      </c>
+      <c r="E25" s="1">
+        <v>0.44500000000000001</v>
+      </c>
+      <c r="F25" s="1">
+        <v>0.73540000000000005</v>
       </c>
       <c r="G25" s="1">
         <v>0.44500000000000001</v>
@@ -1430,22 +1538,22 @@
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>3</v>
-      </c>
-      <c r="B26">
-        <v>3</v>
-      </c>
-      <c r="C26">
-        <v>1</v>
-      </c>
-      <c r="D26">
-        <v>0</v>
-      </c>
-      <c r="E26">
-        <v>2</v>
-      </c>
-      <c r="F26">
-        <v>1</v>
+        <v>0.32979999999999998</v>
+      </c>
+      <c r="B26" s="1">
+        <v>0.32979999999999998</v>
+      </c>
+      <c r="C26" s="1">
+        <v>0.54520000000000002</v>
+      </c>
+      <c r="D26" s="1">
+        <v>0.32979999999999998</v>
+      </c>
+      <c r="E26" s="1">
+        <v>0.32979999999999998</v>
+      </c>
+      <c r="F26" s="1">
+        <v>0.54520000000000002</v>
       </c>
       <c r="G26" s="1">
         <v>0.32979999999999998</v>
@@ -1460,22 +1568,22 @@
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>3</v>
-      </c>
-      <c r="B27">
-        <v>3</v>
-      </c>
-      <c r="C27">
-        <v>1</v>
-      </c>
-      <c r="D27">
-        <v>1</v>
-      </c>
-      <c r="E27">
-        <v>2</v>
-      </c>
-      <c r="F27">
-        <v>0</v>
+        <v>0.36049999999999999</v>
+      </c>
+      <c r="B27" s="1">
+        <v>0.36049999999999999</v>
+      </c>
+      <c r="C27" s="1">
+        <v>0.59589999999999999</v>
+      </c>
+      <c r="D27" s="1">
+        <v>0.36049999999999999</v>
+      </c>
+      <c r="E27" s="1">
+        <v>0.36049999999999999</v>
+      </c>
+      <c r="F27" s="1">
+        <v>0.59589999999999999</v>
       </c>
       <c r="G27" s="1">
         <v>0.36049999999999999</v>
@@ -1490,22 +1598,22 @@
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>3</v>
-      </c>
-      <c r="B28">
-        <v>3</v>
-      </c>
-      <c r="C28">
-        <v>1</v>
-      </c>
-      <c r="D28">
-        <v>0</v>
-      </c>
-      <c r="E28">
-        <v>2</v>
-      </c>
-      <c r="F28">
-        <v>0</v>
+        <v>0.1918</v>
+      </c>
+      <c r="B28" s="1">
+        <v>0.1918</v>
+      </c>
+      <c r="C28" s="1">
+        <v>0.317</v>
+      </c>
+      <c r="D28" s="1">
+        <v>0.1918</v>
+      </c>
+      <c r="E28" s="1">
+        <v>0.1918</v>
+      </c>
+      <c r="F28" s="1">
+        <v>0.317</v>
       </c>
       <c r="G28" s="1">
         <v>0.1918</v>
@@ -1520,22 +1628,22 @@
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>4</v>
-      </c>
-      <c r="B29">
-        <v>4</v>
-      </c>
-      <c r="C29">
-        <v>1</v>
-      </c>
-      <c r="D29">
-        <v>1</v>
-      </c>
-      <c r="E29">
-        <v>2</v>
-      </c>
-      <c r="F29">
-        <v>1</v>
+        <v>1.84E-2</v>
+      </c>
+      <c r="B29" s="1">
+        <v>1.84E-2</v>
+      </c>
+      <c r="C29" s="1">
+        <v>3.0499999999999999E-2</v>
+      </c>
+      <c r="D29" s="1">
+        <v>1.84E-2</v>
+      </c>
+      <c r="E29" s="1">
+        <v>1.84E-2</v>
+      </c>
+      <c r="F29" s="1">
+        <v>3.0499999999999999E-2</v>
       </c>
       <c r="G29" s="1">
         <v>1.84E-2</v>
@@ -1550,22 +1658,22 @@
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>4</v>
-      </c>
-      <c r="B30">
-        <v>4</v>
-      </c>
-      <c r="C30">
-        <v>1</v>
-      </c>
-      <c r="D30">
-        <v>0</v>
-      </c>
-      <c r="E30">
-        <v>2</v>
-      </c>
-      <c r="F30">
-        <v>1</v>
+        <v>1.26E-2</v>
+      </c>
+      <c r="B30" s="1">
+        <v>1.26E-2</v>
+      </c>
+      <c r="C30" s="1">
+        <v>2.0899999999999998E-2</v>
+      </c>
+      <c r="D30" s="1">
+        <v>1.26E-2</v>
+      </c>
+      <c r="E30" s="1">
+        <v>1.26E-2</v>
+      </c>
+      <c r="F30" s="1">
+        <v>2.0899999999999998E-2</v>
       </c>
       <c r="G30" s="1">
         <v>1.26E-2</v>
@@ -1580,22 +1688,22 @@
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>4</v>
-      </c>
-      <c r="B31">
-        <v>4</v>
-      </c>
-      <c r="C31">
-        <v>1</v>
-      </c>
-      <c r="D31">
-        <v>1</v>
-      </c>
-      <c r="E31">
-        <v>2</v>
-      </c>
-      <c r="F31">
-        <v>0</v>
+        <v>1.26E-2</v>
+      </c>
+      <c r="B31" s="1">
+        <v>1.26E-2</v>
+      </c>
+      <c r="C31" s="1">
+        <v>2.0899999999999998E-2</v>
+      </c>
+      <c r="D31" s="1">
+        <v>1.26E-2</v>
+      </c>
+      <c r="E31" s="1">
+        <v>1.26E-2</v>
+      </c>
+      <c r="F31" s="1">
+        <v>2.0899999999999998E-2</v>
       </c>
       <c r="G31" s="1">
         <v>1.26E-2</v>
@@ -1610,22 +1718,22 @@
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32">
-        <v>4</v>
-      </c>
-      <c r="B32">
-        <v>4</v>
-      </c>
-      <c r="C32">
-        <v>1</v>
-      </c>
-      <c r="D32">
-        <v>0</v>
-      </c>
-      <c r="E32">
-        <v>2</v>
-      </c>
-      <c r="F32">
-        <v>0</v>
+        <v>7.7000000000000002E-3</v>
+      </c>
+      <c r="B32" s="1">
+        <v>7.7000000000000002E-3</v>
+      </c>
+      <c r="C32" s="1">
+        <v>1.2699999999999999E-2</v>
+      </c>
+      <c r="D32" s="1">
+        <v>7.7000000000000002E-3</v>
+      </c>
+      <c r="E32" s="1">
+        <v>7.7000000000000002E-3</v>
+      </c>
+      <c r="F32" s="1">
+        <v>1.2699999999999999E-2</v>
       </c>
       <c r="G32" s="1">
         <v>7.7000000000000002E-3</v>
@@ -1640,22 +1748,22 @@
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>6</v>
-      </c>
-      <c r="B33">
-        <v>6</v>
-      </c>
-      <c r="C33">
-        <v>1</v>
-      </c>
-      <c r="D33">
-        <v>1</v>
-      </c>
-      <c r="E33">
-        <v>2</v>
-      </c>
-      <c r="F33">
-        <v>1</v>
+        <v>0.34</v>
+      </c>
+      <c r="B33" s="1">
+        <v>0.34</v>
+      </c>
+      <c r="C33" s="1">
+        <v>0.46</v>
+      </c>
+      <c r="D33" s="1">
+        <v>0.34</v>
+      </c>
+      <c r="E33" s="1">
+        <v>0.34</v>
+      </c>
+      <c r="F33" s="1">
+        <v>0.46</v>
       </c>
       <c r="G33" s="1">
         <v>0.34</v>
@@ -1670,22 +1778,22 @@
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>6</v>
-      </c>
-      <c r="B34">
-        <v>6</v>
-      </c>
-      <c r="C34">
-        <v>1</v>
-      </c>
-      <c r="D34">
-        <v>0</v>
-      </c>
-      <c r="E34">
-        <v>2</v>
-      </c>
-      <c r="F34">
-        <v>1</v>
+        <v>0.255</v>
+      </c>
+      <c r="B34" s="1">
+        <v>0.255</v>
+      </c>
+      <c r="C34" s="1">
+        <v>0.34499999999999997</v>
+      </c>
+      <c r="D34" s="1">
+        <v>0.255</v>
+      </c>
+      <c r="E34" s="1">
+        <v>0.255</v>
+      </c>
+      <c r="F34" s="1">
+        <v>0.34499999999999997</v>
       </c>
       <c r="G34" s="1">
         <v>0.255</v>
@@ -1700,22 +1808,22 @@
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35">
-        <v>6</v>
-      </c>
-      <c r="B35">
-        <v>6</v>
-      </c>
-      <c r="C35">
-        <v>1</v>
-      </c>
-      <c r="D35">
-        <v>1</v>
-      </c>
-      <c r="E35">
-        <v>2</v>
-      </c>
-      <c r="F35">
-        <v>0</v>
+        <v>0.255</v>
+      </c>
+      <c r="B35" s="1">
+        <v>0.255</v>
+      </c>
+      <c r="C35" s="1">
+        <v>0.34499999999999997</v>
+      </c>
+      <c r="D35" s="1">
+        <v>0.255</v>
+      </c>
+      <c r="E35" s="1">
+        <v>0.255</v>
+      </c>
+      <c r="F35" s="1">
+        <v>0.34499999999999997</v>
       </c>
       <c r="G35" s="1">
         <v>0.255</v>
@@ -1730,22 +1838,22 @@
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36">
-        <v>6</v>
-      </c>
-      <c r="B36">
-        <v>6</v>
-      </c>
-      <c r="C36">
-        <v>1</v>
-      </c>
-      <c r="D36">
-        <v>0</v>
-      </c>
-      <c r="E36">
-        <v>2</v>
-      </c>
-      <c r="F36">
-        <v>0</v>
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="B36" s="1">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="C36" s="1">
+        <v>0.115</v>
+      </c>
+      <c r="D36" s="1">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="E36" s="1">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="F36" s="1">
+        <v>0.115</v>
       </c>
       <c r="G36" s="1">
         <v>8.5000000000000006E-2</v>
@@ -1760,22 +1868,22 @@
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37">
-        <v>7</v>
-      </c>
-      <c r="B37">
-        <v>7</v>
-      </c>
-      <c r="C37">
-        <v>1</v>
-      </c>
-      <c r="D37">
-        <v>1</v>
-      </c>
-      <c r="E37">
-        <v>2</v>
-      </c>
-      <c r="F37">
-        <v>1</v>
+        <v>1.15E-2</v>
+      </c>
+      <c r="B37" s="1">
+        <v>1.15E-2</v>
+      </c>
+      <c r="C37" s="1">
+        <v>1.9E-2</v>
+      </c>
+      <c r="D37" s="1">
+        <v>1.15E-2</v>
+      </c>
+      <c r="E37" s="1">
+        <v>1.15E-2</v>
+      </c>
+      <c r="F37" s="1">
+        <v>1.9E-2</v>
       </c>
       <c r="G37" s="1">
         <v>1.15E-2</v>
@@ -1790,22 +1898,22 @@
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38">
-        <v>7</v>
-      </c>
-      <c r="B38">
-        <v>7</v>
-      </c>
-      <c r="C38">
-        <v>1</v>
-      </c>
-      <c r="D38">
-        <v>0</v>
-      </c>
-      <c r="E38">
-        <v>2</v>
-      </c>
-      <c r="F38">
-        <v>1</v>
+        <v>6.6E-3</v>
+      </c>
+      <c r="B38" s="1">
+        <v>6.6E-3</v>
+      </c>
+      <c r="C38" s="1">
+        <v>1.0800000000000001E-2</v>
+      </c>
+      <c r="D38" s="1">
+        <v>6.6E-3</v>
+      </c>
+      <c r="E38" s="1">
+        <v>6.6E-3</v>
+      </c>
+      <c r="F38" s="1">
+        <v>1.0800000000000001E-2</v>
       </c>
       <c r="G38" s="1">
         <v>6.6E-3</v>
@@ -1820,22 +1928,22 @@
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39">
-        <v>7</v>
-      </c>
-      <c r="B39">
-        <v>7</v>
-      </c>
-      <c r="C39">
-        <v>1</v>
-      </c>
-      <c r="D39">
-        <v>1</v>
-      </c>
-      <c r="E39">
-        <v>2</v>
-      </c>
-      <c r="F39">
-        <v>0</v>
+        <v>6.6E-3</v>
+      </c>
+      <c r="B39" s="1">
+        <v>6.6E-3</v>
+      </c>
+      <c r="C39" s="1">
+        <v>1.0800000000000001E-2</v>
+      </c>
+      <c r="D39" s="1">
+        <v>6.6E-3</v>
+      </c>
+      <c r="E39" s="1">
+        <v>6.6E-3</v>
+      </c>
+      <c r="F39" s="1">
+        <v>1.0800000000000001E-2</v>
       </c>
       <c r="G39" s="1">
         <v>6.6E-3</v>
@@ -1850,22 +1958,22 @@
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40">
-        <v>7</v>
-      </c>
-      <c r="B40">
-        <v>7</v>
-      </c>
-      <c r="C40">
-        <v>1</v>
-      </c>
-      <c r="D40">
-        <v>0</v>
-      </c>
-      <c r="E40">
-        <v>2</v>
-      </c>
-      <c r="F40">
-        <v>0</v>
+        <v>2.7000000000000001E-3</v>
+      </c>
+      <c r="B40" s="1">
+        <v>2.7000000000000001E-3</v>
+      </c>
+      <c r="C40" s="1">
+        <v>4.4000000000000003E-3</v>
+      </c>
+      <c r="D40" s="1">
+        <v>2.7000000000000001E-3</v>
+      </c>
+      <c r="E40" s="1">
+        <v>2.7000000000000001E-3</v>
+      </c>
+      <c r="F40" s="1">
+        <v>4.4000000000000003E-3</v>
       </c>
       <c r="G40" s="1">
         <v>2.7000000000000001E-3</v>
@@ -1880,22 +1988,22 @@
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41">
-        <v>9</v>
-      </c>
-      <c r="B41">
-        <v>9</v>
-      </c>
-      <c r="C41">
-        <v>3</v>
-      </c>
-      <c r="D41">
-        <v>1</v>
-      </c>
-      <c r="E41">
-        <v>6</v>
-      </c>
-      <c r="F41">
-        <v>1</v>
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="B41" s="1">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="C41" s="1">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="D41" s="1">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="E41" s="1">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="F41" s="1">
+        <v>4.5999999999999999E-2</v>
       </c>
       <c r="G41" s="1">
         <v>3.4000000000000002E-2</v>
@@ -1910,22 +2018,22 @@
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42">
-        <v>9</v>
-      </c>
-      <c r="B42">
-        <v>9</v>
-      </c>
-      <c r="C42">
-        <v>3</v>
-      </c>
-      <c r="D42">
-        <v>0</v>
-      </c>
-      <c r="E42">
-        <v>6</v>
-      </c>
-      <c r="F42">
-        <v>1</v>
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="B42" s="1">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="C42" s="1">
+        <v>2.3E-2</v>
+      </c>
+      <c r="D42" s="1">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="E42" s="1">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="F42" s="1">
+        <v>2.3E-2</v>
       </c>
       <c r="G42" s="1">
         <v>1.7000000000000001E-2</v>
@@ -1940,22 +2048,22 @@
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43">
-        <v>9</v>
-      </c>
-      <c r="B43">
-        <v>9</v>
-      </c>
-      <c r="C43">
-        <v>3</v>
-      </c>
-      <c r="D43">
-        <v>1</v>
-      </c>
-      <c r="E43">
-        <v>6</v>
-      </c>
-      <c r="F43">
-        <v>0</v>
+        <v>1.49E-2</v>
+      </c>
+      <c r="B43" s="1">
+        <v>1.49E-2</v>
+      </c>
+      <c r="C43" s="1">
+        <v>2.01E-2</v>
+      </c>
+      <c r="D43" s="1">
+        <v>1.49E-2</v>
+      </c>
+      <c r="E43" s="1">
+        <v>1.49E-2</v>
+      </c>
+      <c r="F43" s="1">
+        <v>2.01E-2</v>
       </c>
       <c r="G43" s="1">
         <v>1.49E-2</v>
@@ -1970,22 +2078,22 @@
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A44">
-        <v>9</v>
-      </c>
-      <c r="B44">
-        <v>9</v>
-      </c>
-      <c r="C44">
-        <v>3</v>
-      </c>
-      <c r="D44">
-        <v>0</v>
-      </c>
-      <c r="E44">
-        <v>6</v>
-      </c>
-      <c r="F44">
-        <v>0</v>
+        <v>8.5000000000000006E-3</v>
+      </c>
+      <c r="B44" s="1">
+        <v>8.5000000000000006E-3</v>
+      </c>
+      <c r="C44" s="1">
+        <v>1.15E-2</v>
+      </c>
+      <c r="D44" s="1">
+        <v>8.5000000000000006E-3</v>
+      </c>
+      <c r="E44" s="1">
+        <v>8.5000000000000006E-3</v>
+      </c>
+      <c r="F44" s="1">
+        <v>1.15E-2</v>
       </c>
       <c r="G44" s="1">
         <v>8.5000000000000006E-3</v>
@@ -2000,22 +2108,22 @@
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A45">
-        <v>10</v>
-      </c>
-      <c r="B45">
-        <v>10</v>
-      </c>
-      <c r="C45">
-        <v>8</v>
-      </c>
-      <c r="D45">
-        <v>1</v>
-      </c>
-      <c r="E45">
-        <v>9</v>
-      </c>
-      <c r="F45">
-        <v>1</v>
+        <v>5.9499999999999997E-2</v>
+      </c>
+      <c r="B45" s="1">
+        <v>5.9499999999999997E-2</v>
+      </c>
+      <c r="C45" s="1">
+        <v>8.0500000000000002E-2</v>
+      </c>
+      <c r="D45" s="1">
+        <v>5.9499999999999997E-2</v>
+      </c>
+      <c r="E45" s="1">
+        <v>5.9499999999999997E-2</v>
+      </c>
+      <c r="F45" s="1">
+        <v>8.0500000000000002E-2</v>
       </c>
       <c r="G45" s="1">
         <v>5.9499999999999997E-2</v>
@@ -2030,22 +2138,22 @@
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A46">
-        <v>10</v>
-      </c>
-      <c r="B46">
-        <v>10</v>
-      </c>
-      <c r="C46">
-        <v>8</v>
-      </c>
-      <c r="D46">
-        <v>0</v>
-      </c>
-      <c r="E46">
-        <v>9</v>
-      </c>
-      <c r="F46">
-        <v>1</v>
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="B46" s="1">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="C46" s="1">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="D46" s="1">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="E46" s="1">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="F46" s="1">
+        <v>4.5999999999999999E-2</v>
       </c>
       <c r="G46" s="1">
         <v>3.4000000000000002E-2</v>
@@ -2060,22 +2168,22 @@
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A47">
-        <v>10</v>
-      </c>
-      <c r="B47">
-        <v>10</v>
-      </c>
-      <c r="C47">
-        <v>8</v>
-      </c>
-      <c r="D47">
-        <v>1</v>
-      </c>
-      <c r="E47">
-        <v>9</v>
-      </c>
-      <c r="F47">
-        <v>0</v>
+        <v>3.61E-2</v>
+      </c>
+      <c r="B47" s="1">
+        <v>3.61E-2</v>
+      </c>
+      <c r="C47" s="1">
+        <v>4.8899999999999999E-2</v>
+      </c>
+      <c r="D47" s="1">
+        <v>3.61E-2</v>
+      </c>
+      <c r="E47" s="1">
+        <v>3.61E-2</v>
+      </c>
+      <c r="F47" s="1">
+        <v>4.8899999999999999E-2</v>
       </c>
       <c r="G47" s="1">
         <v>3.61E-2</v>
@@ -2090,22 +2198,22 @@
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48">
-        <v>10</v>
-      </c>
-      <c r="B48">
-        <v>10</v>
-      </c>
-      <c r="C48">
-        <v>8</v>
-      </c>
-      <c r="D48">
-        <v>0</v>
-      </c>
-      <c r="E48">
-        <v>9</v>
-      </c>
-      <c r="F48">
-        <v>0</v>
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="B48" s="1">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="C48" s="1">
+        <v>2.3E-2</v>
+      </c>
+      <c r="D48" s="1">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="E48" s="1">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="F48" s="1">
+        <v>2.3E-2</v>
       </c>
       <c r="G48" s="1">
         <v>1.7000000000000001E-2</v>
@@ -2248,6 +2356,8 @@
         <v>0</v>
       </c>
       <c r="J53" s="7"/>
+      <c r="L53" s="7"/>
+      <c r="M53" s="7"/>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
@@ -2271,6 +2381,9 @@
       <c r="H54" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="J54" s="7"/>
+      <c r="L54" s="7"/>
+      <c r="M54" s="7"/>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B55" t="s">
@@ -2294,6 +2407,9 @@
       <c r="H55" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="J55" s="7"/>
+      <c r="L55" s="7"/>
+      <c r="M55" s="7"/>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B56" t="s">
@@ -2317,6 +2433,7 @@
       <c r="H56" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="J56" s="7"/>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B57" t="s">
@@ -8084,7 +8201,7 @@
   <dimension ref="A1:K47"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:A47"/>
+      <selection activeCell="S34" sqref="S34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8098,51 +8215,53 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1"/>
-      <c r="B1">
-        <v>23</v>
-      </c>
-      <c r="C1">
-        <v>3</v>
-      </c>
-      <c r="D1">
-        <v>3</v>
-      </c>
-      <c r="E1">
-        <v>3</v>
-      </c>
-      <c r="F1">
-        <v>3</v>
-      </c>
-      <c r="G1" s="1">
-        <v>3</v>
-      </c>
-      <c r="H1" s="1">
-        <v>3</v>
+      <c r="A1" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>13</v>
       </c>
       <c r="I1" s="1"/>
       <c r="J1" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>23</v>
+      </c>
+      <c r="B2">
+        <v>23</v>
+      </c>
+      <c r="C2">
         <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2"/>
-      <c r="B2">
-        <v>3</v>
-      </c>
-      <c r="C2" t="str">
-        <f>IFERROR(IF(D2=0,CODE(RIGHT(Input_Toy!#REF!,LEN(Input_Toy!#REF!)-1))-64,CODE(Input_Toy!#REF!)-64),"")</f>
-        <v/>
       </c>
       <c r="D2">
         <v>3</v>
       </c>
-      <c r="E2" t="str">
-        <f>IFERROR(IF(F2=0,CODE(RIGHT(Input_Toy!#REF!,LEN(Input_Toy!#REF!)-1))-64,CODE(Input_Toy!#REF!)-64),"")</f>
-        <v/>
+      <c r="E2">
+        <v>3</v>
       </c>
       <c r="F2">
         <v>3</v>
@@ -8162,7 +8281,9 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3"/>
+      <c r="A3">
+        <v>3</v>
+      </c>
       <c r="B3">
         <v>3</v>
       </c>
@@ -8195,7 +8316,32 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4"/>
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="str">
+        <f>IFERROR(IF(D4=0,CODE(RIGHT(Input_Toy!#REF!,LEN(Input_Toy!#REF!)-1))-64,CODE(Input_Toy!#REF!)-64),"")</f>
+        <v/>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4" t="str">
+        <f>IFERROR(IF(F4=0,CODE(RIGHT(Input_Toy!#REF!,LEN(Input_Toy!#REF!)-1))-64,CODE(Input_Toy!#REF!)-64),"")</f>
+        <v/>
+      </c>
+      <c r="F4">
+        <v>3</v>
+      </c>
+      <c r="G4" s="1">
+        <v>3</v>
+      </c>
+      <c r="H4" s="1">
+        <v>3</v>
+      </c>
       <c r="J4" s="3" t="s">
         <v>5</v>
       </c>
@@ -8217,7 +8363,6 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7"/>
-      <c r="C7" s="6"/>
       <c r="J7" s="4" t="s">
         <v>25</v>
       </c>
@@ -8227,6 +8372,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8"/>
+      <c r="C8" s="6"/>
       <c r="J8" s="4" t="s">
         <v>2</v>
       </c>
@@ -8275,10 +8421,10 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14"/>
-      <c r="D14" s="6"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15"/>
+      <c r="D15" s="6"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16"/>
@@ -8382,5 +8528,6 @@
   <headerFooter alignWithMargins="0">
     <oddFooter>&amp;L&amp;Z&amp;F&amp;A</oddFooter>
   </headerFooter>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added debug (instead of script) to capture returned error/output messages
</commit_message>
<xml_diff>
--- a/testDocumentationRAddin.xlsx
+++ b/testDocumentationRAddin.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1883" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1883" uniqueCount="44">
   <si>
     <t/>
   </si>
@@ -116,9 +116,6 @@
     <t>Absolute Paths in dir or the definition path column are defined by starting with \\ or X:\ (X being a drive letter)</t>
   </si>
   <si>
-    <t>rexec is the full path to an executable being able to run the script in line "script" (usually Rscript.exe). It is only needed when overriding the ExePath in the AppSettings in the Raddin-AddIn-packed.xll.config file.</t>
-  </si>
-  <si>
     <t>When running cmd shell files a special entry "cmd" is used for rexec.</t>
   </si>
   <si>
@@ -126,12 +123,6 @@
   </si>
   <si>
     <t>An area name can be Workbook global or worksheet local, the first Rdefinition area is being taken as the default definition (used for running when not selecting a Rdefinition)</t>
-  </si>
-  <si>
-    <t>1st column: definition types, possible types are rexec, dir, script, arg (R input objects, txt files), res (R output objects, txt files) and diag (R output diagrams, png format)</t>
-  </si>
-  <si>
-    <t>2nd column: definition values, for rexec, dir and script this is simply the path/name of the executable/Rdefinition directory/script.</t>
   </si>
   <si>
     <t>For arg, res and diag these are range names referring to the respective ranges to be taken as arg, res or diag target in the excel workbook.</t>
@@ -156,6 +147,18 @@
   </si>
   <si>
     <t>result:</t>
+  </si>
+  <si>
+    <t>rexec is the full path to an executable, being able to run the script in line "script" (usually Rscript.exe). It is only needed when overriding the ExePath in the AppSettings in the Raddin-AddIn-packed.xll.config file.</t>
+  </si>
+  <si>
+    <t>2nd column: definition values, for rexec, dir and script (debug) this is simply the path/name of the executable/Rdefinition directory/script.</t>
+  </si>
+  <si>
+    <t>1st column: definition types, possible types are rexec, dir, script (put debug here to capture &amp; return error output) , arg (R input objects, txt files), res (R output objects, txt files) and diag (R output diagrams, png format)</t>
+  </si>
+  <si>
+    <t>debug</t>
   </si>
 </sst>
 </file>
@@ -291,20 +294,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>53</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="testdiagram.png"/>
+        <xdr:cNvPr id="3" name="testdiagram.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -323,7 +326,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4810125" y="4095750"/>
+          <a:off x="4010025" y="4048125"/>
           <a:ext cx="4572000" cy="4572000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -353,7 +356,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="testdiagram.png"/>
+        <xdr:cNvPr id="3" name="testdiagram.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -676,7 +679,7 @@
   <dimension ref="A1:O306"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R19" sqref="R19"/>
+      <selection activeCell="M19" sqref="M19:O23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -710,7 +713,7 @@
         <v>13</v>
       </c>
       <c r="J1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
@@ -740,7 +743,7 @@
       </c>
       <c r="I2" s="7"/>
       <c r="J2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
@@ -770,7 +773,7 @@
       </c>
       <c r="I3" s="7"/>
       <c r="J3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
@@ -800,7 +803,7 @@
       </c>
       <c r="I4" s="7"/>
       <c r="J4" s="8" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
@@ -830,7 +833,7 @@
       </c>
       <c r="I5" s="7"/>
       <c r="J5" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
@@ -860,7 +863,7 @@
       </c>
       <c r="I6" s="7"/>
       <c r="J6" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
@@ -977,7 +980,7 @@
       </c>
       <c r="I10" s="7"/>
       <c r="J10" s="7" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
@@ -1007,7 +1010,7 @@
       </c>
       <c r="I11" s="7"/>
       <c r="J11" s="7" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
@@ -1037,7 +1040,7 @@
       </c>
       <c r="I12" s="7"/>
       <c r="J12" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L12" s="7"/>
       <c r="M12" s="7"/>
@@ -1069,7 +1072,7 @@
       </c>
       <c r="I13" s="7"/>
       <c r="J13" s="7" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="L13" s="7"/>
       <c r="M13" s="7"/>
@@ -1133,7 +1136,7 @@
       </c>
       <c r="I15" s="7"/>
       <c r="J15" s="7" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="L15" s="7"/>
       <c r="M15" s="7"/>
@@ -1165,7 +1168,7 @@
       </c>
       <c r="I16" s="7"/>
       <c r="J16" s="7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
@@ -1195,7 +1198,7 @@
       </c>
       <c r="I17" s="7"/>
       <c r="J17" s="7" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.2">
@@ -8157,7 +8160,7 @@
   <dimension ref="A1:K47"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S34" sqref="S34"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8172,7 +8175,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>14</v>
@@ -8230,7 +8233,7 @@
       </c>
       <c r="I2" s="1"/>
       <c r="J2" s="3" t="s">
-        <v>1</v>
+        <v>43</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>8</v>

</xml_diff>